<commit_message>
Modify Excel Form Version 2 20190609
</commit_message>
<xml_diff>
--- a/CSharp/Code/2_TransferCoordinate/Z_tmplate/7A0004_圖號座標轉換_圖號座標轉換.xlsx
+++ b/CSharp/Code/2_TransferCoordinate/Z_tmplate/7A0004_圖號座標轉換_圖號座標轉換.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="8040" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="三維坐標轉換-e-GNSS2017轉TWD97-2019_04" sheetId="1" r:id="rId1"/>
-    <sheet name="TWD97轉TWD67" sheetId="2" r:id="rId2"/>
+    <sheet name="三維坐標轉換-e-GNSS2017轉TWD97-2019_04" sheetId="20" r:id="rId1"/>
+    <sheet name="TWD97轉TWD67" sheetId="21" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
+  <si>
+    <t>經辦人:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    ☐符合                 ☐未符合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>課長:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>點號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,6 +155,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>配合辦理管線定位測量、管線施作及圖資更新維護作業明細表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ＤＣＩＳ:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>施工號碼:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>TWD97</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -159,6 +183,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>正高</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -356,6 +384,10 @@
   </si>
   <si>
     <t>M9703BE0786</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測量技術士簽名:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -363,7 +395,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -379,21 +411,138 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -402,9 +551,48 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,31 +882,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -726,7 +914,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>2551732.1779999998</v>
@@ -755,7 +943,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>2551741.0690000001</v>
@@ -784,7 +972,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>2551751.8679999998</v>
@@ -813,7 +1001,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>2551769.497</v>
@@ -842,7 +1030,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>2551769.4950000001</v>
@@ -871,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>2551789.0249999999</v>
@@ -900,7 +1088,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>2551804.2069999999</v>
@@ -929,7 +1117,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>2551821.8250000002</v>
@@ -958,7 +1146,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>2551844.3139999998</v>
@@ -987,7 +1175,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>2551874.9300000002</v>
@@ -1016,7 +1204,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>2551889.3820000002</v>
@@ -1045,7 +1233,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <v>2551913.7030000002</v>
@@ -1074,7 +1262,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>2551915.7110000001</v>
@@ -1103,7 +1291,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>2551927.2579999999</v>
@@ -1132,7 +1320,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>2551947.284</v>
@@ -1161,7 +1349,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>2551948.949</v>
@@ -1190,7 +1378,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>2551956.3939999999</v>
@@ -1219,7 +1407,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>2551964.14</v>
@@ -1248,7 +1436,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>2551985.1839999999</v>
@@ -1277,7 +1465,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <v>2551999.6189999999</v>
@@ -1306,7 +1494,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C22">
         <v>2551999.656</v>
@@ -1335,7 +1523,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>2551861.3130000001</v>
@@ -1364,7 +1552,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>2551832.4849999999</v>
@@ -1393,7 +1581,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>2551767.676</v>
@@ -1425,747 +1613,893 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="7.5" customWidth="1"/>
+    <col min="6" max="6" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2551732.41</v>
+      </c>
+      <c r="C6" s="12">
+        <v>168659.26300000001</v>
+      </c>
+      <c r="D6" s="12">
+        <v>3.556</v>
+      </c>
+      <c r="E6" s="12">
+        <v>23.724</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="12">
+        <v>2551940.3838379201</v>
+      </c>
+      <c r="H6" s="12">
+        <v>167832.21062097099</v>
+      </c>
+      <c r="I6" s="12">
+        <v>3.556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="12">
+        <v>2551741.3020000001</v>
+      </c>
+      <c r="C7" s="12">
+        <v>168626.886</v>
+      </c>
+      <c r="D7" s="12">
+        <v>3.516</v>
+      </c>
+      <c r="E7" s="12">
+        <v>23.683</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="12">
+        <v>2551949.2759113102</v>
+      </c>
+      <c r="H7" s="12">
+        <v>167799.83406450599</v>
+      </c>
+      <c r="I7" s="12">
+        <v>3.516</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="12">
+        <v>2551752.1009999998</v>
+      </c>
+      <c r="C8" s="12">
+        <v>168589.617</v>
+      </c>
+      <c r="D8" s="12">
+        <v>3.6080000000000001</v>
+      </c>
+      <c r="E8" s="12">
+        <v>23.774000000000001</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="12">
+        <v>2551960.0749870599</v>
+      </c>
+      <c r="H8" s="12">
+        <v>167762.565571382</v>
+      </c>
+      <c r="I8" s="12">
+        <v>3.6080000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="12">
+        <v>2551769.7310000001</v>
+      </c>
+      <c r="C9" s="12">
+        <v>168531.83100000001</v>
+      </c>
+      <c r="D9" s="12">
+        <v>3.5529999999999999</v>
+      </c>
+      <c r="E9" s="12">
+        <v>23.718</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="12">
+        <v>2551977.7050907998</v>
+      </c>
+      <c r="H9" s="12">
+        <v>167704.780351522</v>
+      </c>
+      <c r="I9" s="12">
+        <v>3.5529999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="12">
+        <v>2551769.7289999998</v>
+      </c>
+      <c r="C10" s="12">
+        <v>168531.83199999999</v>
+      </c>
+      <c r="D10" s="12">
+        <v>3.556</v>
+      </c>
+      <c r="E10" s="12">
+        <v>23.721</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="12">
+        <v>2551977.70309082</v>
+      </c>
+      <c r="H10" s="12">
+        <v>167704.78135152001</v>
+      </c>
+      <c r="I10" s="12">
+        <v>3.556</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2551789.2590000001</v>
+      </c>
+      <c r="C11" s="12">
+        <v>168463.035</v>
+      </c>
+      <c r="D11" s="12">
+        <v>3.6709999999999998</v>
+      </c>
+      <c r="E11" s="12">
+        <v>23.834</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="12">
+        <v>2551997.2332369299</v>
+      </c>
+      <c r="H11" s="12">
+        <v>167635.98528982999</v>
+      </c>
+      <c r="I11" s="12">
+        <v>3.6709999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="12">
+        <v>2551804.4419999998</v>
+      </c>
+      <c r="C12" s="12">
+        <v>168412.13200000001</v>
+      </c>
+      <c r="D12" s="12">
+        <v>3.629</v>
+      </c>
+      <c r="E12" s="12">
+        <v>23.79</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="12">
+        <v>2552012.41633368</v>
+      </c>
+      <c r="H12" s="12">
+        <v>167585.08297930899</v>
+      </c>
+      <c r="I12" s="12">
+        <v>3.629</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="12">
+        <v>2551822.06</v>
+      </c>
+      <c r="C13" s="12">
+        <v>168353.42300000001</v>
+      </c>
+      <c r="D13" s="12">
+        <v>3.637</v>
+      </c>
+      <c r="E13" s="12">
+        <v>23.797000000000001</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="12">
+        <v>2552030.0344436201</v>
+      </c>
+      <c r="H13" s="12">
+        <v>167526.37477382401</v>
+      </c>
+      <c r="I13" s="12">
+        <v>3.637</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="12">
+        <v>2551844.5499999998</v>
+      </c>
+      <c r="C14" s="12">
+        <v>168277.15599999999</v>
+      </c>
+      <c r="D14" s="12">
+        <v>3.7080000000000002</v>
+      </c>
+      <c r="E14" s="12">
+        <v>23.866</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="12">
+        <v>2552052.5245925901</v>
+      </c>
+      <c r="H14" s="12">
+        <v>167450.10880854301</v>
+      </c>
+      <c r="I14" s="12">
+        <v>3.7080000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="12">
+        <v>2551875.1669999999</v>
+      </c>
+      <c r="C15" s="12">
+        <v>168174.383</v>
+      </c>
+      <c r="D15" s="12">
+        <v>3.7109999999999999</v>
+      </c>
+      <c r="E15" s="12">
+        <v>23.866</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="12">
+        <v>2552083.1417885101</v>
+      </c>
+      <c r="H15" s="12">
+        <v>167347.337200843</v>
+      </c>
+      <c r="I15" s="12">
+        <v>3.7109999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="12">
+        <v>2551889.6189999999</v>
+      </c>
+      <c r="C16" s="12">
+        <v>168126.71599999999</v>
+      </c>
+      <c r="D16" s="12">
+        <v>3.7320000000000002</v>
+      </c>
+      <c r="E16" s="12">
+        <v>23.885999999999999</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="12">
+        <v>2552097.5938754901</v>
+      </c>
+      <c r="H16" s="12">
+        <v>167299.67084496401</v>
+      </c>
+      <c r="I16" s="12">
+        <v>3.7320000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="12">
+        <v>2551913.9410000001</v>
+      </c>
+      <c r="C17" s="12">
+        <v>168045.51800000001</v>
+      </c>
+      <c r="D17" s="12">
+        <v>3.7429999999999999</v>
+      </c>
+      <c r="E17" s="12">
+        <v>23.895</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="12">
+        <v>2552121.91602823</v>
+      </c>
+      <c r="H17" s="12">
+        <v>167218.47394411699</v>
+      </c>
+      <c r="I17" s="12">
+        <v>3.7429999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="12">
+        <v>2551915.949</v>
+      </c>
+      <c r="C18" s="12">
+        <v>168042.546</v>
+      </c>
+      <c r="D18" s="12">
+        <v>3.746</v>
+      </c>
+      <c r="E18" s="12">
+        <v>23.898</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="12">
+        <v>2552123.9240165101</v>
+      </c>
+      <c r="H18" s="12">
+        <v>167215.501977059</v>
+      </c>
+      <c r="I18" s="12">
+        <v>3.746</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="12">
+        <v>2551927.497</v>
+      </c>
+      <c r="C19" s="12">
+        <v>168000.236</v>
+      </c>
+      <c r="D19" s="12">
+        <v>3.7280000000000002</v>
+      </c>
+      <c r="E19" s="12">
+        <v>23.878</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="12">
+        <v>2552135.4721135302</v>
+      </c>
+      <c r="H19" s="12">
+        <v>167173.192557136</v>
+      </c>
+      <c r="I19" s="12">
+        <v>3.7280000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="12">
+        <v>2551947.523</v>
+      </c>
+      <c r="C20" s="12">
+        <v>167932.36300000001</v>
+      </c>
+      <c r="D20" s="12">
+        <v>3.5009999999999999</v>
+      </c>
+      <c r="E20" s="12">
+        <v>23.649000000000001</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="12">
+        <v>2552155.4982459298</v>
+      </c>
+      <c r="H20" s="12">
+        <v>167105.32047790001</v>
+      </c>
+      <c r="I20" s="12">
+        <v>3.5009999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="12">
+        <v>2551949.1880000001</v>
+      </c>
+      <c r="C21" s="12">
+        <v>167929.40599999999</v>
+      </c>
+      <c r="D21" s="12">
+        <v>3.5329999999999999</v>
+      </c>
+      <c r="E21" s="12">
+        <v>23.681000000000001</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="12">
+        <v>2552157.1632394199</v>
+      </c>
+      <c r="H21" s="12">
+        <v>167102.363512846</v>
+      </c>
+      <c r="I21" s="12">
+        <v>3.5329999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="12">
+        <v>2551956.6340000001</v>
+      </c>
+      <c r="C22" s="12">
+        <v>167901.54199999999</v>
+      </c>
+      <c r="D22" s="12">
+        <v>3.8290000000000002</v>
+      </c>
+      <c r="E22" s="12">
+        <v>23.975999999999999</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="12">
+        <v>2552164.6093057799</v>
+      </c>
+      <c r="H22" s="12">
+        <v>167074.49989590401</v>
+      </c>
+      <c r="I22" s="12">
+        <v>3.8290000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="12">
+        <v>2551964.38</v>
+      </c>
+      <c r="C23" s="12">
+        <v>167896.24100000001</v>
+      </c>
+      <c r="D23" s="12">
+        <v>3.6850000000000001</v>
+      </c>
+      <c r="E23" s="12">
+        <v>23.832000000000001</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="12">
+        <v>2552172.35522037</v>
+      </c>
+      <c r="H23" s="12">
+        <v>167069.198927505</v>
+      </c>
+      <c r="I23" s="12">
+        <v>3.6850000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="12">
+        <v>2551985.4249999998</v>
+      </c>
+      <c r="C24" s="12">
+        <v>167803.39300000001</v>
+      </c>
+      <c r="D24" s="12">
+        <v>3.8330000000000002</v>
+      </c>
+      <c r="E24" s="12">
+        <v>23.977</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="12">
+        <v>2552193.4004998398</v>
+      </c>
+      <c r="H24" s="12">
+        <v>166976.35222848601</v>
+      </c>
+      <c r="I24" s="12">
+        <v>3.8330000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="12">
+        <v>2551999.86</v>
+      </c>
+      <c r="C25" s="12">
+        <v>167758.97200000001</v>
+      </c>
+      <c r="D25" s="12">
+        <v>3.7330000000000001</v>
+      </c>
+      <c r="E25" s="12">
+        <v>23.876999999999999</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="12">
+        <v>2552207.8355659102</v>
+      </c>
+      <c r="H25" s="12">
+        <v>166931.93182243701</v>
+      </c>
+      <c r="I25" s="12">
+        <v>3.7330000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="12">
+        <v>2551999.8969999999</v>
+      </c>
+      <c r="C26" s="12">
+        <v>167755.42000000001</v>
+      </c>
+      <c r="D26" s="12">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="E26" s="12">
+        <v>23.879000000000001</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="12">
+        <v>2552207.8725884999</v>
+      </c>
+      <c r="H26" s="12">
+        <v>166928.37987721601</v>
+      </c>
+      <c r="I26" s="12">
+        <v>3.7360000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="12">
+        <v>2551861.5499999998</v>
+      </c>
+      <c r="C27" s="12">
+        <v>168220.20699999999</v>
+      </c>
+      <c r="D27" s="12">
+        <v>3.7240000000000002</v>
+      </c>
+      <c r="E27" s="12">
+        <v>23.88</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="12">
+        <v>2552069.5247006202</v>
+      </c>
+      <c r="H27" s="12">
+        <v>167393.16057982601</v>
+      </c>
+      <c r="I27" s="12">
+        <v>3.7240000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="12">
+        <v>2551832.7209999999</v>
+      </c>
+      <c r="C28" s="12">
+        <v>168316.851</v>
+      </c>
+      <c r="D28" s="12">
+        <v>3.6339999999999999</v>
+      </c>
+      <c r="E28" s="12">
+        <v>23.792999999999999</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="12">
+        <v>2552040.69551697</v>
+      </c>
+      <c r="H28" s="12">
+        <v>167489.803270804</v>
+      </c>
+      <c r="I28" s="12">
+        <v>3.6339999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="12">
+        <v>2551767.91</v>
+      </c>
+      <c r="C29" s="12">
+        <v>168534.696</v>
+      </c>
+      <c r="D29" s="12">
+        <v>3.58</v>
+      </c>
+      <c r="E29" s="12">
+        <v>23.745000000000001</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="12">
+        <v>2551975.8841003198</v>
+      </c>
+      <c r="H29" s="12">
+        <v>167707.64531901799</v>
+      </c>
+      <c r="I29" s="12">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3">
-        <v>2551732.41</v>
-      </c>
-      <c r="C3">
-        <v>168659.26300000001</v>
-      </c>
-      <c r="D3">
-        <v>3.556</v>
-      </c>
-      <c r="E3">
-        <v>23.724</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3">
-        <v>2551940.3838379201</v>
-      </c>
-      <c r="H3">
-        <v>167832.21062097099</v>
-      </c>
-      <c r="I3">
-        <v>3.556</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4">
-        <v>2551741.3020000001</v>
-      </c>
-      <c r="C4">
-        <v>168626.886</v>
-      </c>
-      <c r="D4">
-        <v>3.516</v>
-      </c>
-      <c r="E4">
-        <v>23.683</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4">
-        <v>2551949.2759113102</v>
-      </c>
-      <c r="H4">
-        <v>167799.83406450599</v>
-      </c>
-      <c r="I4">
-        <v>3.516</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5">
-        <v>2551752.1009999998</v>
-      </c>
-      <c r="C5">
-        <v>168589.617</v>
-      </c>
-      <c r="D5">
-        <v>3.6080000000000001</v>
-      </c>
-      <c r="E5">
-        <v>23.774000000000001</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5">
-        <v>2551960.0749870599</v>
-      </c>
-      <c r="H5">
-        <v>167762.565571382</v>
-      </c>
-      <c r="I5">
-        <v>3.6080000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6">
-        <v>2551769.7310000001</v>
-      </c>
-      <c r="C6">
-        <v>168531.83100000001</v>
-      </c>
-      <c r="D6">
-        <v>3.5529999999999999</v>
-      </c>
-      <c r="E6">
-        <v>23.718</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6">
-        <v>2551977.7050907998</v>
-      </c>
-      <c r="H6">
-        <v>167704.780351522</v>
-      </c>
-      <c r="I6">
-        <v>3.5529999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7">
-        <v>2551769.7289999998</v>
-      </c>
-      <c r="C7">
-        <v>168531.83199999999</v>
-      </c>
-      <c r="D7">
-        <v>3.556</v>
-      </c>
-      <c r="E7">
-        <v>23.721</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7">
-        <v>2551977.70309082</v>
-      </c>
-      <c r="H7">
-        <v>167704.78135152001</v>
-      </c>
-      <c r="I7">
-        <v>3.556</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8">
-        <v>2551789.2590000001</v>
-      </c>
-      <c r="C8">
-        <v>168463.035</v>
-      </c>
-      <c r="D8">
-        <v>3.6709999999999998</v>
-      </c>
-      <c r="E8">
-        <v>23.834</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8">
-        <v>2551997.2332369299</v>
-      </c>
-      <c r="H8">
-        <v>167635.98528982999</v>
-      </c>
-      <c r="I8">
-        <v>3.6709999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9">
-        <v>2551804.4419999998</v>
-      </c>
-      <c r="C9">
-        <v>168412.13200000001</v>
-      </c>
-      <c r="D9">
-        <v>3.629</v>
-      </c>
-      <c r="E9">
-        <v>23.79</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9">
-        <v>2552012.41633368</v>
-      </c>
-      <c r="H9">
-        <v>167585.08297930899</v>
-      </c>
-      <c r="I9">
-        <v>3.629</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10">
-        <v>2551822.06</v>
-      </c>
-      <c r="C10">
-        <v>168353.42300000001</v>
-      </c>
-      <c r="D10">
-        <v>3.637</v>
-      </c>
-      <c r="E10">
-        <v>23.797000000000001</v>
-      </c>
-      <c r="F10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10">
-        <v>2552030.0344436201</v>
-      </c>
-      <c r="H10">
-        <v>167526.37477382401</v>
-      </c>
-      <c r="I10">
-        <v>3.637</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11">
-        <v>2551844.5499999998</v>
-      </c>
-      <c r="C11">
-        <v>168277.15599999999</v>
-      </c>
-      <c r="D11">
-        <v>3.7080000000000002</v>
-      </c>
-      <c r="E11">
-        <v>23.866</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11">
-        <v>2552052.5245925901</v>
-      </c>
-      <c r="H11">
-        <v>167450.10880854301</v>
-      </c>
-      <c r="I11">
-        <v>3.7080000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12">
-        <v>2551875.1669999999</v>
-      </c>
-      <c r="C12">
-        <v>168174.383</v>
-      </c>
-      <c r="D12">
-        <v>3.7109999999999999</v>
-      </c>
-      <c r="E12">
-        <v>23.866</v>
-      </c>
-      <c r="F12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12">
-        <v>2552083.1417885101</v>
-      </c>
-      <c r="H12">
-        <v>167347.337200843</v>
-      </c>
-      <c r="I12">
-        <v>3.7109999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13">
-        <v>2551889.6189999999</v>
-      </c>
-      <c r="C13">
-        <v>168126.71599999999</v>
-      </c>
-      <c r="D13">
-        <v>3.7320000000000002</v>
-      </c>
-      <c r="E13">
-        <v>23.885999999999999</v>
-      </c>
-      <c r="F13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13">
-        <v>2552097.5938754901</v>
-      </c>
-      <c r="H13">
-        <v>167299.67084496401</v>
-      </c>
-      <c r="I13">
-        <v>3.7320000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14">
-        <v>2551913.9410000001</v>
-      </c>
-      <c r="C14">
-        <v>168045.51800000001</v>
-      </c>
-      <c r="D14">
-        <v>3.7429999999999999</v>
-      </c>
-      <c r="E14">
-        <v>23.895</v>
-      </c>
-      <c r="F14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14">
-        <v>2552121.91602823</v>
-      </c>
-      <c r="H14">
-        <v>167218.47394411699</v>
-      </c>
-      <c r="I14">
-        <v>3.7429999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15">
-        <v>2551915.949</v>
-      </c>
-      <c r="C15">
-        <v>168042.546</v>
-      </c>
-      <c r="D15">
-        <v>3.746</v>
-      </c>
-      <c r="E15">
-        <v>23.898</v>
-      </c>
-      <c r="F15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15">
-        <v>2552123.9240165101</v>
-      </c>
-      <c r="H15">
-        <v>167215.501977059</v>
-      </c>
-      <c r="I15">
-        <v>3.746</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16">
-        <v>2551927.497</v>
-      </c>
-      <c r="C16">
-        <v>168000.236</v>
-      </c>
-      <c r="D16">
-        <v>3.7280000000000002</v>
-      </c>
-      <c r="E16">
-        <v>23.878</v>
-      </c>
-      <c r="F16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16">
-        <v>2552135.4721135302</v>
-      </c>
-      <c r="H16">
-        <v>167173.192557136</v>
-      </c>
-      <c r="I16">
-        <v>3.7280000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17">
-        <v>2551947.523</v>
-      </c>
-      <c r="C17">
-        <v>167932.36300000001</v>
-      </c>
-      <c r="D17">
-        <v>3.5009999999999999</v>
-      </c>
-      <c r="E17">
-        <v>23.649000000000001</v>
-      </c>
-      <c r="F17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17">
-        <v>2552155.4982459298</v>
-      </c>
-      <c r="H17">
-        <v>167105.32047790001</v>
-      </c>
-      <c r="I17">
-        <v>3.5009999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18">
-        <v>2551949.1880000001</v>
-      </c>
-      <c r="C18">
-        <v>167929.40599999999</v>
-      </c>
-      <c r="D18">
-        <v>3.5329999999999999</v>
-      </c>
-      <c r="E18">
-        <v>23.681000000000001</v>
-      </c>
-      <c r="F18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18">
-        <v>2552157.1632394199</v>
-      </c>
-      <c r="H18">
-        <v>167102.363512846</v>
-      </c>
-      <c r="I18">
-        <v>3.5329999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19">
-        <v>2551956.6340000001</v>
-      </c>
-      <c r="C19">
-        <v>167901.54199999999</v>
-      </c>
-      <c r="D19">
-        <v>3.8290000000000002</v>
-      </c>
-      <c r="E19">
-        <v>23.975999999999999</v>
-      </c>
-      <c r="F19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19">
-        <v>2552164.6093057799</v>
-      </c>
-      <c r="H19">
-        <v>167074.49989590401</v>
-      </c>
-      <c r="I19">
-        <v>3.8290000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20">
-        <v>2551964.38</v>
-      </c>
-      <c r="C20">
-        <v>167896.24100000001</v>
-      </c>
-      <c r="D20">
-        <v>3.6850000000000001</v>
-      </c>
-      <c r="E20">
-        <v>23.832000000000001</v>
-      </c>
-      <c r="F20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20">
-        <v>2552172.35522037</v>
-      </c>
-      <c r="H20">
-        <v>167069.198927505</v>
-      </c>
-      <c r="I20">
-        <v>3.6850000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21">
-        <v>2551985.4249999998</v>
-      </c>
-      <c r="C21">
-        <v>167803.39300000001</v>
-      </c>
-      <c r="D21">
-        <v>3.8330000000000002</v>
-      </c>
-      <c r="E21">
-        <v>23.977</v>
-      </c>
-      <c r="F21" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21">
-        <v>2552193.4004998398</v>
-      </c>
-      <c r="H21">
-        <v>166976.35222848601</v>
-      </c>
-      <c r="I21">
-        <v>3.8330000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22">
-        <v>2551999.86</v>
-      </c>
-      <c r="C22">
-        <v>167758.97200000001</v>
-      </c>
-      <c r="D22">
-        <v>3.7330000000000001</v>
-      </c>
-      <c r="E22">
-        <v>23.876999999999999</v>
-      </c>
-      <c r="F22" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22">
-        <v>2552207.8355659102</v>
-      </c>
-      <c r="H22">
-        <v>166931.93182243701</v>
-      </c>
-      <c r="I22">
-        <v>3.7330000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23">
-        <v>2551999.8969999999</v>
-      </c>
-      <c r="C23">
-        <v>167755.42000000001</v>
-      </c>
-      <c r="D23">
-        <v>3.7360000000000002</v>
-      </c>
-      <c r="E23">
-        <v>23.879000000000001</v>
-      </c>
-      <c r="F23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23">
-        <v>2552207.8725884999</v>
-      </c>
-      <c r="H23">
-        <v>166928.37987721601</v>
-      </c>
-      <c r="I23">
-        <v>3.7360000000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24">
-        <v>2551861.5499999998</v>
-      </c>
-      <c r="C24">
-        <v>168220.20699999999</v>
-      </c>
-      <c r="D24">
-        <v>3.7240000000000002</v>
-      </c>
-      <c r="E24">
-        <v>23.88</v>
-      </c>
-      <c r="F24" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24">
-        <v>2552069.5247006202</v>
-      </c>
-      <c r="H24">
-        <v>167393.16057982601</v>
-      </c>
-      <c r="I24">
-        <v>3.7240000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25">
-        <v>2551832.7209999999</v>
-      </c>
-      <c r="C25">
-        <v>168316.851</v>
-      </c>
-      <c r="D25">
-        <v>3.6339999999999999</v>
-      </c>
-      <c r="E25">
-        <v>23.792999999999999</v>
-      </c>
-      <c r="F25" t="s">
-        <v>80</v>
-      </c>
-      <c r="G25">
-        <v>2552040.69551697</v>
-      </c>
-      <c r="H25">
-        <v>167489.803270804</v>
-      </c>
-      <c r="I25">
-        <v>3.6339999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26">
-        <v>2551767.91</v>
-      </c>
-      <c r="C26">
-        <v>168534.696</v>
-      </c>
-      <c r="D26">
-        <v>3.58</v>
-      </c>
-      <c r="E26">
-        <v>23.745000000000001</v>
-      </c>
-      <c r="F26" t="s">
-        <v>82</v>
-      </c>
-      <c r="G26">
-        <v>2551975.8841003198</v>
-      </c>
-      <c r="H26">
-        <v>167707.64531901799</v>
-      </c>
-      <c r="I26">
-        <v>3.58</v>
-      </c>
-    </row>
+      <c r="H35" s="7"/>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="11"/>
+    </row>
+    <row r="37" spans="1:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>